<commit_message>
more values and edits, will finish tomorrow morning
</commit_message>
<xml_diff>
--- a/Data/CCJ_quantified values.xlsx
+++ b/Data/CCJ_quantified values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larapesceares/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larapesceares/CCJ/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{32171604-EC50-FD49-9583-AC5ECB3C10B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FC1FAB-A3EE-CD47-97BA-9D3FE5A0DB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26460" windowHeight="18360" xr2:uid="{B2B1E421-E324-4B4D-ACA9-CCF9679130E2}"/>
+    <workbookView xWindow="-9480" yWindow="-27820" windowWidth="32540" windowHeight="15920" xr2:uid="{B2B1E421-E324-4B4D-ACA9-CCF9679130E2}"/>
   </bookViews>
   <sheets>
     <sheet name="CCJ_quantified values" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>Component name</t>
   </si>
@@ -78,36 +78,12 @@
     <t>10-year value to detainee</t>
   </si>
   <si>
-    <t>reduced lifetime earnings</t>
-  </si>
-  <si>
     <t>long term</t>
   </si>
   <si>
     <t>FED study</t>
   </si>
   <si>
-    <t>increased health burden</t>
-  </si>
-  <si>
-    <t>reduced life expectancy</t>
-  </si>
-  <si>
-    <t>Value of freedom</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
-  <si>
-    <t>Statutory compensations for wrongful inprisonment</t>
-  </si>
-  <si>
-    <t>dollar by 1 year in prison</t>
-  </si>
-  <si>
-    <t>Reduced chances in the labor market</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -244,6 +220,30 @@
   </si>
   <si>
     <t>input</t>
+  </si>
+  <si>
+    <t>−1,710</t>
+  </si>
+  <si>
+    <t>−5,623</t>
+  </si>
+  <si>
+    <t>reduced income</t>
+  </si>
+  <si>
+    <t>−3,677</t>
+  </si>
+  <si>
+    <t>10-year cost to government</t>
+  </si>
+  <si>
+    <t>Short-term cost to government</t>
+  </si>
+  <si>
+    <t>Direct Funding for CCJ (2018)</t>
+  </si>
+  <si>
+    <t>dollars</t>
   </si>
 </sst>
 </file>
@@ -743,13 +743,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1126,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995123B1-1625-034D-9BEA-A8F37EC1EE44}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,6 +1148,7 @@
     <col min="2" max="2" width="62.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="11" max="12" width="13.33203125" customWidth="1"/>
     <col min="14" max="14" width="25.6640625" customWidth="1"/>
   </cols>
@@ -1150,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1159,16 +1170,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -1177,25 +1188,25 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="M1" t="s">
         <v>7</v>
       </c>
       <c r="N1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -1203,195 +1214,345 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>0.3</v>
-      </c>
-      <c r="K2">
-        <v>0.5</v>
+        <v>15</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2018</v>
       </c>
       <c r="M2" t="s">
         <v>13</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="P5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>50000</v>
-      </c>
-      <c r="J6">
-        <v>80000</v>
-      </c>
-      <c r="K6">
-        <v>200000</v>
-      </c>
-      <c r="M6" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7">
-        <v>0.25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>60.37</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6">
+        <v>60.37</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>0.61</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.71</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10" s="6">
+        <v>11</v>
+      </c>
+      <c r="I10" s="6">
+        <v>33</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10">
+        <v>2011</v>
+      </c>
+      <c r="O10" t="s">
+        <v>40</v>
       </c>
       <c r="P10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
+      </c>
+      <c r="G11">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="6">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12">
+        <v>-99.44</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1399,295 +1560,120 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="G13">
-        <v>60.37</v>
-      </c>
-      <c r="H13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13">
-        <v>60.37</v>
-      </c>
-      <c r="J13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" t="s">
-        <v>47</v>
+        <v>-11</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6">
+        <v>11</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>2022</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
       </c>
       <c r="O13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="P13" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G14">
-        <v>0.61</v>
-      </c>
-      <c r="H14">
-        <v>0.61</v>
-      </c>
-      <c r="I14" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14">
-        <v>0.71</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="F14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="5">
+        <v>-249634</v>
+      </c>
+      <c r="H14" s="7">
+        <v>178920</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="7">
+        <v>249634</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2021</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="P14" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>55</v>
-      </c>
-      <c r="R14" t="s">
-        <v>54</v>
+      <c r="P14" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15">
-        <v>11</v>
-      </c>
-      <c r="H15">
-        <v>11</v>
-      </c>
-      <c r="I15">
-        <v>33</v>
-      </c>
-      <c r="J15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15">
-        <v>2011</v>
-      </c>
-      <c r="O15" t="s">
-        <v>48</v>
-      </c>
-      <c r="P15" t="s">
-        <v>49</v>
+      <c r="A15" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="A16" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="H16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="J16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-      <c r="N16" t="s">
-        <v>59</v>
-      </c>
-      <c r="O16" t="s">
-        <v>60</v>
-      </c>
-      <c r="P16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
-      <c r="F17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17">
-        <v>99.44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18">
-        <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18">
-        <v>2022</v>
-      </c>
-      <c r="M18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O18" t="s">
-        <v>65</v>
-      </c>
-      <c r="P18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="5">
-        <v>249634</v>
-      </c>
-      <c r="H19" s="5">
-        <v>178920</v>
-      </c>
-      <c r="I19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="5">
-        <v>249634</v>
-      </c>
-      <c r="L19">
-        <v>2021</v>
-      </c>
-      <c r="M19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O19" t="s">
-        <v>65</v>
-      </c>
-      <c r="P19" t="s">
-        <v>66</v>
+      <c r="G17" s="9">
+        <v>448677628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>